<commit_message>
Ajoute dans le tableau de bord
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelie/switchdrive/GREP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelie/Documents/GitHub/WavContact/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E781BBBA-F949-A845-B7A1-8700988AC6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDBCA02-354E-0D49-A0F4-02A653299FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Cours de mise en pratique avec Steeve</t>
+  </si>
+  <si>
+    <t>Réunion de groupe</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1530,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1681,9 +1684,15 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="8"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="8">
+        <v>44487</v>
+      </c>
+      <c r="C12" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="8"/>
@@ -6613,7 +6622,7 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
maj journal de bord Constantin
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelie/Documents/GitHub/WavContact/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/constantin/Documents/GitHub/WavContact/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDBCA02-354E-0D49-A0F4-02A653299FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D929338-D910-5148-B2BB-A85A410206F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -259,6 +259,18 @@
   </si>
   <si>
     <t>Réunion de groupe</t>
+  </si>
+  <si>
+    <t>0h30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversation avec Waview pour maj </t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>Création des maquettes v1</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1542,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -6622,8 +6634,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6755,14 +6767,26 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="36">
+        <v>44479</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="14"/>
+      <c r="B9" s="36">
+        <v>44485</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="36"/>

</xml_diff>

<commit_message>
MAJ journal de bord (Angela)
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coral\OneDrive\Documents\GitHub\WavContact\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B404604-DA98-41AE-BE55-E7F15B08C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A43DB-5B7F-40C6-91C0-F6B4AB164D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="240" windowWidth="18400" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -295,6 +295,21 @@
   </si>
   <si>
     <t>Modification du planning</t>
+  </si>
+  <si>
+    <t>Recherche de nouveaux risques (Waview et nous)</t>
+  </si>
+  <si>
+    <t>Mise à jour document vision selon retour lors de la réunion A1</t>
+  </si>
+  <si>
+    <t>Prise de note pour la présentation A1</t>
+  </si>
+  <si>
+    <t>Vérification + correction du PV (réunion A1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remplissage sprint + backlog </t>
   </si>
 </sst>
 </file>
@@ -722,20 +737,110 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF504A3B"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFE39202"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bookman Old Style"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE1AE"/>
+          <bgColor rgb="FFFEE1AE"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -841,38 +946,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF504A3B"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
@@ -907,39 +980,6 @@
         <b/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFE39202"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -963,31 +1003,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Bookman Old Style"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEE1AE"/>
-          <bgColor rgb="FFFEE1AE"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1318,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D23">
-  <autoFilter ref="B2:D23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D25">
+  <autoFilter ref="B2:D25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DATE" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DURÉE" dataDxfId="13"/>
@@ -1348,9 +1363,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D43" totalsRowCount="1">
   <autoFilter ref="B2:D42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ÉVÉNEMENT" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="7" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ÉVÉNEMENT" dataDxfId="6" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1360,9 +1375,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau2" displayName="Tableau2" ref="B2:D14">
   <autoFilter ref="B2:D14" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="DATE" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DURÉE" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ÉVÉNEMENT" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="DATE" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DURÉE" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ÉVÉNEMENT" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1599,11 +1614,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2788,10 +2803,10 @@
     <tabColor rgb="FFD8B1CB"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2805,11 +2820,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3022,32 +3037,70 @@
       </c>
     </row>
     <row r="19" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="45"/>
+      <c r="B19" s="17">
+        <v>44487</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="20" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="45"/>
+      <c r="B20" s="17">
+        <v>44491</v>
+      </c>
+      <c r="C20" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="45"/>
+      <c r="B21" s="17">
+        <v>44493</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="45"/>
-    </row>
-    <row r="23" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B22" s="17">
+        <v>44494</v>
+      </c>
+      <c r="C22" s="18">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="17">
+        <v>44497</v>
+      </c>
+      <c r="C23" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="43"/>
+    </row>
+    <row r="25" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="17"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="14"/>
+    </row>
     <row r="26" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4039,6 +4092,8 @@
     <row r="1014" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1015" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1016" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1017" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1018" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
@@ -4059,7 +4114,7 @@
   </sheetPr>
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -4074,11 +4129,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -5327,8 +5382,8 @@
   </sheetPr>
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5342,11 +5397,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -6802,8 +6857,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6817,11 +6872,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>

</xml_diff>

<commit_message>
MAJ journal de bord ( ajout ordre du jour A2)
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A43DB-5B7F-40C6-91C0-F6B4AB164D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA360F4-7807-4BAF-9727-838ABC7064F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="240" windowWidth="18400" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t xml:space="preserve">Remplissage sprint + backlog </t>
+  </si>
+  <si>
+    <t>Création ordre du jour pour la réunion A2</t>
   </si>
 </sst>
 </file>
@@ -756,96 +759,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF504A3B"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFE39202"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Bookman Old Style"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEE1AE"/>
-          <bgColor rgb="FFFEE1AE"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
@@ -946,6 +859,38 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF504A3B"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
@@ -980,6 +925,39 @@
         <b/>
         <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFE39202"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -1003,6 +981,31 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bookman Old Style"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE1AE"/>
+          <bgColor rgb="FFFEE1AE"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1333,8 +1336,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D25">
-  <autoFilter ref="B2:D25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D26">
+  <autoFilter ref="B2:D26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DATE" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DURÉE" dataDxfId="13"/>
@@ -1363,9 +1366,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D43" totalsRowCount="1">
   <autoFilter ref="B2:D42" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ÉVÉNEMENT" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="ÉVÉNEMENT" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1375,9 +1378,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau2" displayName="Tableau2" ref="B2:D14">
   <autoFilter ref="B2:D14" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="DATE" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DURÉE" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ÉVÉNEMENT" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="DATE" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DURÉE" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ÉVÉNEMENT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2803,10 +2806,10 @@
     <tabColor rgb="FFD8B1CB"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1019"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3082,26 +3085,36 @@
     </row>
     <row r="23" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="17">
+        <v>44494</v>
+      </c>
+      <c r="C23" s="18">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17">
         <v>44497</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C24" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D24" s="43" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="43"/>
-    </row>
-    <row r="25" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="43"/>
+    </row>
+    <row r="26" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="17"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="14"/>
+    </row>
     <row r="27" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4094,6 +4107,7 @@
     <row r="1016" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1017" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1018" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1019" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
MAJ journal de bord
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coral\OneDrive\Documents\GitHub\WavContact\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091DC218-00D8-4245-9317-CCA491CD5213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D631A4F-8C06-409C-9E36-BE3EB13DFF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Suite de l'écriture des sprints et du backlog et finalisation du document de vision avec Angela</t>
+  </si>
+  <si>
+    <t>Suite de l'écriture des sprints et du backlog et finalisation du document de vision avec Coralie</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1614,7 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2817,8 +2820,8 @@
   </sheetPr>
   <dimension ref="A1:Z1021"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3144,7 +3147,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5434,7 +5437,7 @@
   <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
maj des horaires de constantin
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aurelie/Documents/GitHub/WavContact/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/constantin/Documents/GitHub/WavContact/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389E37A-BD3C-1D47-9CA9-8E3D463CE50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D695D49-3C34-2944-AE2F-E17FCA48D4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>Débrifing de la réunion A2 en groupe</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Finalisation des maquettes</t>
+  </si>
+  <si>
+    <t>0h30</t>
+  </si>
+  <si>
+    <t>Mise au propre du PV + prise de rendez-vous avec Waview</t>
+  </si>
+  <si>
+    <t>Mise en page du PV avec la reunion de Waview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunion avec le mandant </t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1429,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau2" displayName="Tableau2" ref="B2:D14">
-  <autoFilter ref="B2:D14" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau2" displayName="Tableau2" ref="B2:D16">
+  <autoFilter ref="B2:D16" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="DATE" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DURÉE" dataDxfId="1"/>
@@ -1638,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1836,9 +1854,15 @@
       </c>
     </row>
     <row r="16" spans="1:26" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="8"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="10"/>
+      <c r="B16" s="8">
+        <v>44508</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="8"/>
@@ -4215,7 +4239,7 @@
   </sheetPr>
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -5496,7 +5520,7 @@
   <dimension ref="A1:Z1014"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B39" sqref="B39:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7022,8 +7046,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7221,19 +7245,37 @@
       </c>
     </row>
     <row r="14" spans="1:26" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="35"/>
+      <c r="B14" s="38">
+        <v>44502</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:26" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="38">
+        <v>44506</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:26" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="38">
+        <v>44508</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="17" spans="2:4" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="36"/>

</xml_diff>

<commit_message>
Mise à jour partie Angela
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083263BA-AB73-4D74-B440-2CC244290659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60079506-7322-4870-BD87-0CA9A44C0DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="168">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>Suite Forms sur Visual Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du sprint 4 </t>
+  </si>
+  <si>
+    <t>Mise à jour du product bqckolg</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1830,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D45">
-  <autoFilter ref="B2:D45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D48">
+  <autoFilter ref="B2:D48" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DATE" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DURÉE" dataDxfId="14"/>
@@ -3362,10 +3368,10 @@
     <tabColor rgb="FFD8B1CB"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1038"/>
+  <dimension ref="A1:Z1041"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:D44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3881,14 +3887,44 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="90"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="70"/>
-    </row>
-    <row r="46" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:4" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="90">
+        <v>44545</v>
+      </c>
+      <c r="C45" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D45" s="94" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="90">
+        <v>44545</v>
+      </c>
+      <c r="C46" s="72">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D46" s="94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="90">
+        <v>44545</v>
+      </c>
+      <c r="C47" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D47" s="94" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="90"/>
+      <c r="C48" s="72"/>
+      <c r="D48" s="70"/>
+    </row>
     <row r="49" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4879,6 +4915,9 @@
     <row r="1036" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1037" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1038" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1039" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1040" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1041" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Ajout des mails dans le dossier
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E308D540-8EC6-4912-BEF1-303012613BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0B8475-F77E-4B81-A37F-7858C6026D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="205">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -2389,7 +2389,7 @@
   </sheetPr>
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -6960,7 +6960,7 @@
   </sheetPr>
   <dimension ref="A1:Z1043"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A60" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -7818,9 +7818,15 @@
       </c>
     </row>
     <row r="74" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="115"/>
-      <c r="C74" s="116"/>
-      <c r="D74" s="51"/>
+      <c r="B74" s="73">
+        <v>44600</v>
+      </c>
+      <c r="C74" s="74">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D74" s="55" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="75" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="68"/>

</xml_diff>

<commit_message>
Modification de l'étude d'opportunité
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0B8475-F77E-4B81-A37F-7858C6026D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A7658E-05A1-41D9-98FA-C3BE097EE05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="206">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>Renommage des documents et gestion des documents</t>
+  </si>
+  <si>
+    <t>Mise à jour de l'étude d'opportunité</t>
   </si>
 </sst>
 </file>
@@ -2150,8 +2153,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D75" totalsRowCount="1" totalsRowDxfId="9">
-  <autoFilter ref="B2:D74" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D76" totalsRowCount="1" totalsRowDxfId="9">
+  <autoFilter ref="B2:D75" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="7" totalsRowDxfId="1"/>
@@ -6958,10 +6961,10 @@
     <tabColor rgb="FFFEE1AE"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1043"/>
+  <dimension ref="A1:Z1044"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7828,15 +7831,25 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="68"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="55"/>
+    <row r="75" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="73">
+        <v>44600</v>
+      </c>
+      <c r="C75" s="74">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D75" s="55" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="76" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="114"/>
-    </row>
-    <row r="77" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B76" s="68"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="55"/>
+    </row>
+    <row r="77" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="114"/>
+    </row>
     <row r="78" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8803,6 +8816,7 @@
     <row r="1041" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1042" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1043" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1044" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Màj assurance qualité et classement
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coral\OneDrive\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EE1771-2776-4696-9262-CDC761279B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4AA23-8ACB-4E59-B608-D7E298A5B21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="214">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>Modification du script BDD et de sa modélisation  pour WavMap</t>
+  </si>
+  <si>
+    <t>Mise à jour du document d'assurance qualité et renommage des documents</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
     <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF504A3B"/>
@@ -856,18 +859,6 @@
       <color rgb="FFE39202"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Bookman Old Style"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFE39202"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1160,7 +1151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1536,10 +1527,10 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1547,12 +1538,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2192,8 +2177,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D81" totalsRowCount="1" totalsRowDxfId="9">
-  <autoFilter ref="B2:D80" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D82" totalsRowCount="1" totalsRowDxfId="9">
+  <autoFilter ref="B2:D81" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="8" totalsRowDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="7" totalsRowDxfId="1"/>
@@ -7024,10 +7009,10 @@
     <tabColor rgb="FFFEE1AE"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1049"/>
+  <dimension ref="A1:Z1050"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:D79"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7928,10 +7913,10 @@
       </c>
     </row>
     <row r="78" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="129">
+      <c r="B78" s="125">
         <v>44613</v>
       </c>
-      <c r="C78" s="130">
+      <c r="C78" s="126">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D78" s="55" t="s">
@@ -7939,10 +7924,10 @@
       </c>
     </row>
     <row r="79" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="129">
+      <c r="B79" s="125">
         <v>44613</v>
       </c>
-      <c r="C79" s="130">
+      <c r="C79" s="126">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D79" s="55" t="s">
@@ -7950,19 +7935,35 @@
       </c>
     </row>
     <row r="80" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="125"/>
-      <c r="C80" s="126"/>
-      <c r="D80" s="51"/>
-    </row>
-    <row r="81" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="67"/>
-      <c r="C81" s="56"/>
-      <c r="D81" s="55"/>
+      <c r="B80" s="125">
+        <v>44613</v>
+      </c>
+      <c r="C80" s="126">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D80" s="55" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="125">
+        <v>44614</v>
+      </c>
+      <c r="C81" s="126">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D81" s="55" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="82" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="108"/>
-    </row>
-    <row r="83" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B82" s="67"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="55"/>
+    </row>
+    <row r="83" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="108"/>
+    </row>
     <row r="84" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8929,6 +8930,7 @@
     <row r="1047" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1048" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1049" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1050" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Mise à jour sprint, backlog, journal de bord
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F0A54A-6146-4365-B95A-9D39A513A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D597A-B296-4AA0-9DEA-FCA4DE2E1219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -1784,17 +1784,17 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2679,11 +2679,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3999,8 +3999,8 @@
   </sheetPr>
   <dimension ref="A1:Y1070"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView showGridLines="0" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4014,11 +4014,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -4937,10 +4937,10 @@
       <c r="B83" s="70">
         <v>44650</v>
       </c>
-      <c r="C83" s="129">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D83" s="130" t="s">
+      <c r="C83" s="127">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D83" s="128" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5970,11 +5970,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -7655,7 +7655,7 @@
   </sheetPr>
   <dimension ref="A1:Z1079"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A106" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B110" sqref="B110:D112"/>
     </sheetView>
   </sheetViews>
@@ -7670,11 +7670,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -9953,11 +9953,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>

</xml_diff>

<commit_message>
Création pdf pv et ajout jdb
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coral\OneDrive\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D011F3D7-BDE5-415B-A66D-BB926870FDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6609702-2403-4500-8A41-BCF7C25794C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commun" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="305">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>Post-réunion A4</t>
+  </si>
+  <si>
+    <t>Vérification et modification du PV A4</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1875,6 +1878,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2387,8 +2396,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D93" tableBorderDxfId="13">
-  <autoFilter ref="B2:D93" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:D94" tableBorderDxfId="13">
+  <autoFilter ref="B2:D94" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DATE" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DURÉE" dataDxfId="11"/>
@@ -2414,8 +2423,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D122" totalsRowShown="0">
-  <autoFilter ref="B2:D122" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D124" totalsRowShown="0">
+  <autoFilter ref="B2:D124" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="5" totalsRowDxfId="4"/>
@@ -4007,10 +4016,10 @@
     <tabColor rgb="FFD8B1CB"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y1079"/>
+  <dimension ref="A1:Y1080"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5053,12 +5062,22 @@
         <v>298</v>
       </c>
     </row>
-    <row r="93" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="70"/>
-      <c r="C93" s="56"/>
-      <c r="D93" s="100"/>
-    </row>
-    <row r="94" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="70">
+        <v>44677</v>
+      </c>
+      <c r="C93" s="133">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D93" s="134" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="70"/>
+      <c r="C94" s="56"/>
+      <c r="D94" s="100"/>
+    </row>
     <row r="95" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="96" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="97" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6044,6 +6063,7 @@
     <row r="1077" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1078" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1079" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1080" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
@@ -7824,10 +7844,10 @@
     <tabColor rgb="FFFEE1AE"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1088"/>
+  <dimension ref="A1:Z1090"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView showGridLines="0" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123:C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9211,12 +9231,32 @@
       </c>
     </row>
     <row r="122" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="127"/>
-      <c r="C122" s="80"/>
-      <c r="D122" s="55"/>
-    </row>
-    <row r="123" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B122" s="129">
+        <v>44677</v>
+      </c>
+      <c r="C122" s="130">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D122" s="128" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="129">
+        <v>44677</v>
+      </c>
+      <c r="C123" s="130">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D123" s="128" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="127"/>
+      <c r="C124" s="80"/>
+      <c r="D124" s="55"/>
+    </row>
     <row r="125" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="126" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10181,6 +10221,8 @@
     <row r="1086" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1087" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1088" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1089" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1090" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Modification de la modélisation et BDD WavMap
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6733229-24ED-443F-AE81-A4C7F547970C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B34BA9-108D-4FFC-BF0C-226197821B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="373">
   <si>
     <t>AGENDA COMMUN</t>
   </si>
@@ -1152,6 +1152,9 @@
   </si>
   <si>
     <t>Continuation du code et ajoutes de tous les commentaires</t>
+  </si>
+  <si>
+    <t>Mise à jour de la BDD et de la modélisation BDD de WavMap</t>
   </si>
 </sst>
 </file>
@@ -2166,20 +2169,20 @@
     <xf numFmtId="164" fontId="36" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="37" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="37" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2719,8 +2722,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D154" totalsRowShown="0">
-  <autoFilter ref="B2:D154" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau1" displayName="Tableau1" ref="B2:D155" totalsRowShown="0">
+  <autoFilter ref="B2:D155" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DURÉE" dataDxfId="5" totalsRowDxfId="4"/>
@@ -2973,11 +2976,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -4370,11 +4373,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -6711,11 +6714,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -8671,10 +8674,10 @@
     <tabColor rgb="FFFEE1AE"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1105"/>
+  <dimension ref="A1:Z1106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153:D153"/>
+      <selection activeCell="C154" sqref="B154:C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8688,11 +8691,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -10405,16 +10408,26 @@
       <c r="C153" s="140">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="D153" s="145" t="s">
+      <c r="D153" s="143" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="154" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="143"/>
-      <c r="C154" s="144"/>
-      <c r="D154" s="145"/>
-    </row>
-    <row r="155" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" spans="2:4" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="139">
+        <v>44710</v>
+      </c>
+      <c r="C154" s="140">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D154" s="138" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B155" s="141"/>
+      <c r="C155" s="142"/>
+      <c r="D155" s="143"/>
+    </row>
     <row r="156" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="157" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="158" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11365,6 +11378,7 @@
     <row r="1103" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1104" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1105" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1106" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
@@ -11401,11 +11415,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>

</xml_diff>

<commit_message>
ajout horaire Journal de bord
</commit_message>
<xml_diff>
--- a/Documents/0_Journal_de_bord.xlsx
+++ b/Documents/0_Journal_de_bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Constantin\Documents\GitHub\WavContact\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA593BDD-0484-4F60-A29F-0D528F6CD05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7448684-B1A4-4562-909C-BDE90C7FA0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="17777" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1194,7 +1194,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="hh&quot;h&quot;mm"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -2171,22 +2171,22 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="34" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="34" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2981,11 +2981,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -4378,11 +4378,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -6752,11 +6752,11 @@
   <sheetData>
     <row r="1" spans="1:25" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -8789,11 +8789,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -11516,7 +11516,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11532,11 +11532,11 @@
   <sheetData>
     <row r="1" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -12065,9 +12065,9 @@
       <c r="D45" s="69" t="s">
         <v>325</v>
       </c>
-      <c r="G45" s="143">
+      <c r="G45" s="141">
         <f>SUM(C45:C60)</f>
-        <v>2.145833333333333</v>
+        <v>2.2291666666666665</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -12214,24 +12214,24 @@
       </c>
     </row>
     <row r="59" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="140">
+      <c r="B59" s="138">
         <v>44712</v>
       </c>
-      <c r="C59" s="141">
-        <v>0.125</v>
-      </c>
-      <c r="D59" s="142" t="s">
+      <c r="C59" s="139">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D59" s="140" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="140">
+      <c r="B60" s="138">
         <v>44713</v>
       </c>
-      <c r="C60" s="141">
+      <c r="C60" s="139">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D60" s="142" t="s">
+      <c r="D60" s="140" t="s">
         <v>382</v>
       </c>
     </row>

</xml_diff>